<commit_message>
add: new functionality for automatic creation of the Spearman correlation matrix for bank indicators and a stress-test rules system
</commit_message>
<xml_diff>
--- a/output_bank_indicators/bank_indicators_table.xlsx
+++ b/output_bank_indicators/bank_indicators_table.xlsx
@@ -695,10 +695,10 @@
         <v>0.14</v>
       </c>
       <c r="J2" t="n">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
       <c r="K2" t="n">
-        <v>0.52</v>
+        <v>1.31</v>
       </c>
       <c r="L2" t="n">
         <v>0.16</v>
@@ -866,10 +866,10 @@
         <v>0.11</v>
       </c>
       <c r="J3" t="n">
-        <v>0.39</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="K3" t="n">
-        <v>1.06</v>
+        <v>2.51</v>
       </c>
       <c r="L3" t="n">
         <v>0.24</v>
@@ -1040,7 +1040,7 @@
         <v>0.15</v>
       </c>
       <c r="K4" t="n">
-        <v>3.51</v>
+        <v>5.56</v>
       </c>
       <c r="L4" t="n">
         <v>0.01</v>
@@ -1208,10 +1208,10 @@
         <v>0.11</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.06</v>
       </c>
       <c r="K5" t="n">
-        <v>0.73</v>
+        <v>1.25</v>
       </c>
       <c r="L5" t="n">
         <v>0.16</v>
@@ -1379,10 +1379,10 @@
         <v>0.12</v>
       </c>
       <c r="J6" t="n">
-        <v>0.12</v>
+        <v>0.03</v>
       </c>
       <c r="K6" t="n">
-        <v>0.55</v>
+        <v>1.17</v>
       </c>
       <c r="L6" t="n">
         <v>0.32</v>
@@ -1685,10 +1685,10 @@
         <v>0.23</v>
       </c>
       <c r="J8" t="n">
-        <v>0.67</v>
+        <v>0.08</v>
       </c>
       <c r="K8" t="n">
-        <v>1.26</v>
+        <v>2.34</v>
       </c>
       <c r="L8" t="n">
         <v>0.39</v>
@@ -1856,10 +1856,10 @@
         <v>0.41</v>
       </c>
       <c r="J9" t="n">
-        <v>0.22</v>
+        <v>0.09</v>
       </c>
       <c r="K9" t="n">
-        <v>1.5</v>
+        <v>3.46</v>
       </c>
       <c r="L9" t="n">
         <v>0.25</v>
@@ -2027,10 +2027,10 @@
         <v>0.13</v>
       </c>
       <c r="J10" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="K10" t="n">
-        <v>0.14</v>
+        <v>0.38</v>
       </c>
       <c r="L10" t="n">
         <v>0.11</v>

</xml_diff>